<commit_message>
multiply params by a random value
</commit_message>
<xml_diff>
--- a/test/input/scenarios/mobi31test/scoringParametersIT.xlsx
+++ b/test/input/scenarios/mobi31test/scoringParametersIT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\40_Projekte\20231019_MATSimba2\EAP\IT_Tests_MLFlow\sim\custom_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\matsim-sbb\test\input\scenarios\mobi31test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45773C-1945-47DA-9F2C-52C7DCE0CD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353E7CA8-9F37-48F2-948B-DA9186C94F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="674" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="25170" windowHeight="15720" tabRatio="674" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScoringParams" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="67">
   <si>
     <t>adaptation time</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Dieses Excel ist nur für den Integration Test !!!</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -242,12 +245,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
-    <numFmt numFmtId="174" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -604,8 +607,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,15 +663,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,22 +689,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,21 +716,21 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -780,10 +783,10 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,13 +798,13 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,7 +816,7 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="16" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -837,40 +840,40 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="16" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,13 +909,13 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -928,17 +931,17 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1400,13 +1403,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1438,21 +1441,21 @@
       <c r="A1" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
+      <c r="N1" s="135"/>
       <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1553,37 +1556,37 @@
       </c>
       <c r="C4" s="118"/>
       <c r="D4" s="92">
-        <v>-0.15</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E4" s="93">
-        <v>-0.94</v>
+        <v>-0.7</v>
       </c>
       <c r="F4" s="125">
         <v>0</v>
       </c>
       <c r="G4" s="92">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="H4" s="92">
         <v>0</v>
       </c>
       <c r="I4" s="132">
-        <v>-0.45</v>
+        <v>-0.43</v>
       </c>
       <c r="J4" s="93">
-        <v>-0.35</v>
+        <v>-0.26</v>
       </c>
       <c r="K4" s="93">
-        <v>-0.15</v>
+        <v>-0.06</v>
       </c>
       <c r="L4" s="129">
-        <v>-0.5</v>
+        <v>-0.17</v>
       </c>
       <c r="M4" s="92">
-        <v>0.25</v>
+        <v>0.02</v>
       </c>
       <c r="N4" s="94">
-        <v>-0.55000000000000004</v>
+        <v>-0.24</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="21" t="s">
@@ -1605,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="131">
-        <v>-1.5E-5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="89">
         <v>0</v>
@@ -1645,39 +1648,37 @@
       </c>
       <c r="C6" s="118"/>
       <c r="D6" s="52">
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="E6" s="53">
-        <v>-3.14</v>
+        <v>-0.79</v>
       </c>
       <c r="F6" s="87">
-        <v>-0.35</v>
+        <v>-0.17</v>
       </c>
       <c r="G6" s="52">
-        <f>-0.08</f>
-        <v>-0.08</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="H6" s="52">
-        <v>-2.52</v>
+        <v>-0.31</v>
       </c>
       <c r="I6" s="53">
-        <v>-1.75</v>
+        <v>-0.22</v>
       </c>
       <c r="J6" s="53">
-        <v>-3.14</v>
+        <v>-0.09</v>
       </c>
       <c r="K6" s="53">
-        <v>-0.9</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="L6" s="86">
-        <v>-3.5</v>
+        <v>-3.25</v>
       </c>
       <c r="M6" s="52">
-        <f>-1.14+0.5</f>
-        <v>-0.6399999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="N6" s="53">
-        <v>-1.5899999999999999</v>
+        <v>-0.7</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="69" t="s">
@@ -1699,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="126">
-        <v>-3.4200000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="G7" s="89">
         <v>0</v>
@@ -1726,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="13"/>
-      <c r="P7" s="134" t="s">
+      <c r="P7" s="136" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1734,19 +1735,39 @@
       <c r="A8" s="16"/>
       <c r="B8" s="119"/>
       <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
+      <c r="D8" s="40" t="s">
+        <v>66</v>
+      </c>
       <c r="E8" s="41"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="41"/>
+      <c r="F8" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="130" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>66</v>
+      </c>
       <c r="O8" s="13"/>
-      <c r="P8" s="134"/>
+      <c r="P8" s="136"/>
     </row>
     <row r="9" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -1756,21 +1777,37 @@
         <v>32</v>
       </c>
       <c r="C9" s="80">
-        <v>-0.1</v>
+        <v>-0.04</v>
       </c>
       <c r="D9" s="95"/>
       <c r="E9" s="96"/>
       <c r="F9" s="96"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="99"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="96"/>
+      <c r="G9" s="97" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="96" t="s">
+        <v>66</v>
+      </c>
       <c r="O9" s="14"/>
-      <c r="P9" s="135"/>
+      <c r="P9" s="137"/>
     </row>
     <row r="10" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -1780,22 +1817,35 @@
         <v>1</v>
       </c>
       <c r="C10" s="57">
-        <v>0.12000000000000005</v>
+        <v>0.08</v>
       </c>
       <c r="D10" s="100"/>
       <c r="E10" s="101"/>
       <c r="F10" s="127"/>
       <c r="G10" s="100">
-        <f>C10</f>
-        <v>0.12000000000000005</v>
-      </c>
-      <c r="H10" s="100"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="101"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H10" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="102" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="101" t="s">
+        <v>66</v>
+      </c>
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,14 +1861,30 @@
       <c r="D11" s="98"/>
       <c r="E11" s="96"/>
       <c r="F11" s="96"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="96"/>
+      <c r="G11" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="96" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="96" t="s">
+        <v>66</v>
+      </c>
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1829,19 +1895,35 @@
         <v>0</v>
       </c>
       <c r="C12" s="54">
-        <v>-2.2799999999999998</v>
+        <v>-0.68</v>
       </c>
       <c r="D12" s="100"/>
       <c r="E12" s="101"/>
       <c r="F12" s="127"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="101"/>
+      <c r="G12" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="102" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="101" t="s">
+        <v>66</v>
+      </c>
       <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,14 +1939,30 @@
       <c r="D13" s="100"/>
       <c r="E13" s="101"/>
       <c r="F13" s="127"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="101"/>
+      <c r="G13" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="102" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="101" t="s">
+        <v>66</v>
+      </c>
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1875,19 +1973,35 @@
         <v>5</v>
       </c>
       <c r="C14" s="54">
-        <v>2.2799999999999998</v>
+        <v>1.18</v>
       </c>
       <c r="D14" s="100"/>
       <c r="E14" s="101"/>
       <c r="F14" s="127"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="101"/>
+      <c r="G14" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="102" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" s="101" t="s">
+        <v>66</v>
+      </c>
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1898,51 +2012,40 @@
         <v>3</v>
       </c>
       <c r="C15" s="84">
-        <v>0.16400000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="D15" s="103">
-        <f>C15</f>
-        <v>0.16400000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="104">
-        <f t="shared" ref="E15:N15" si="0">D15</f>
-        <v>0.16400000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="F15" s="104">
-        <f>D15</f>
-        <v>0.16400000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="G15" s="103">
-        <f>E15</f>
-        <v>0.16400000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="H15" s="103">
-        <f t="shared" si="0"/>
-        <v>0.16400000000000001</v>
+        <v>0</v>
       </c>
       <c r="I15" s="104">
-        <f t="shared" si="0"/>
-        <v>0.16400000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="J15" s="104">
-        <f t="shared" si="0"/>
-        <v>0.16400000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K15" s="104">
-        <f t="shared" si="0"/>
-        <v>0.16400000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="L15" s="105">
-        <f>J15</f>
-        <v>0.16400000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="M15" s="103">
-        <f>K15</f>
-        <v>0.16400000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="N15" s="104">
-        <f t="shared" si="0"/>
-        <v>0.16400000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="O15" s="14"/>
     </row>
@@ -1959,14 +2062,30 @@
       <c r="D16" s="106"/>
       <c r="E16" s="108"/>
       <c r="F16" s="107"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="108"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="106"/>
-      <c r="N16" s="107"/>
+      <c r="G16" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="107" t="s">
+        <v>66</v>
+      </c>
       <c r="O16" s="67"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1977,22 +2096,35 @@
         <v>46</v>
       </c>
       <c r="C17" s="78">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="D17" s="109"/>
       <c r="E17" s="111"/>
       <c r="F17" s="110"/>
       <c r="G17" s="109">
-        <f>C17</f>
-        <v>0.05</v>
-      </c>
-      <c r="H17" s="109"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="111"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="110"/>
+        <v>0.03</v>
+      </c>
+      <c r="H17" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="110" t="s">
+        <v>66</v>
+      </c>
       <c r="O17" s="67"/>
     </row>
     <row r="18" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2003,22 +2135,35 @@
         <v>42</v>
       </c>
       <c r="C18" s="85">
-        <v>-0.47499999999999998</v>
+        <v>-0.16</v>
       </c>
       <c r="D18" s="109"/>
       <c r="E18" s="111"/>
       <c r="F18" s="110"/>
       <c r="G18" s="109">
-        <f>C18</f>
-        <v>-0.47499999999999998</v>
-      </c>
-      <c r="H18" s="109"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="109"/>
-      <c r="N18" s="110"/>
+        <v>-0.46</v>
+      </c>
+      <c r="H18" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="110" t="s">
+        <v>66</v>
+      </c>
       <c r="O18" s="67"/>
     </row>
     <row r="19" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2034,14 +2179,30 @@
       <c r="D19" s="109"/>
       <c r="E19" s="111"/>
       <c r="F19" s="110"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
-      <c r="K19" s="111"/>
-      <c r="L19" s="110"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="110"/>
+      <c r="G19" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="111" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="110" t="s">
+        <v>66</v>
+      </c>
       <c r="O19" s="67"/>
     </row>
     <row r="20" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2052,19 +2213,35 @@
         <v>50</v>
       </c>
       <c r="C20" s="79">
-        <v>-0.8</v>
+        <v>-0.36</v>
       </c>
       <c r="D20" s="112"/>
       <c r="E20" s="114"/>
       <c r="F20" s="113"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="114"/>
-      <c r="K20" s="114"/>
-      <c r="L20" s="113"/>
-      <c r="M20" s="112"/>
-      <c r="N20" s="113"/>
+      <c r="G20" s="112" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="112" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="114" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" s="114" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="114" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="113" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="112" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20" s="113" t="s">
+        <v>66</v>
+      </c>
       <c r="O20" s="67"/>
     </row>
     <row r="21" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -2086,9 +2263,6 @@
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O23" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2309,11 +2483,11 @@
       <c r="P4" s="71"/>
       <c r="Q4" s="62">
         <f>D4+ScoringParams!D4</f>
-        <v>-0.15</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="R4" s="63">
         <f>E4+ScoringParams!E4</f>
-        <v>-0.94</v>
+        <v>-0.7</v>
       </c>
       <c r="S4" s="48">
         <f>F4+ScoringParams!F4</f>
@@ -2321,7 +2495,7 @@
       </c>
       <c r="T4" s="63">
         <f>G4+ScoringParams!G4</f>
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="U4" s="63">
         <f>H4+ScoringParams!H4</f>
@@ -2329,27 +2503,27 @@
       </c>
       <c r="V4" s="63">
         <f>I4+ScoringParams!I4</f>
-        <v>-0.45</v>
+        <v>-0.43</v>
       </c>
       <c r="W4" s="63">
         <f>J4+ScoringParams!J4</f>
-        <v>-0.35</v>
+        <v>-0.26</v>
       </c>
       <c r="X4" s="48">
         <f>K4+ScoringParams!K4</f>
-        <v>-0.15</v>
+        <v>-0.06</v>
       </c>
       <c r="Y4" s="48">
         <f>L4+ScoringParams!L4</f>
-        <v>-0.5</v>
+        <v>-0.17</v>
       </c>
       <c r="Z4" s="48">
         <f>M4+ScoringParams!M4</f>
-        <v>0.25</v>
+        <v>0.02</v>
       </c>
       <c r="AA4" s="49">
         <f>N4+ScoringParams!N4</f>
-        <v>-0.55000000000000004</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -2404,7 +2578,7 @@
       </c>
       <c r="S5" s="50">
         <f>F5+ScoringParams!F5</f>
-        <v>-1.5E-5</v>
+        <v>0</v>
       </c>
       <c r="T5" s="59">
         <f>G5+ScoringParams!G5</f>
@@ -2483,47 +2657,47 @@
       <c r="P6" s="75"/>
       <c r="Q6" s="42">
         <f>D6+ScoringParams!D6</f>
-        <v>-1.25</v>
+        <v>-0.44</v>
       </c>
       <c r="R6" s="41">
         <f>E6+ScoringParams!E6</f>
-        <v>-3.14</v>
+        <v>-0.79</v>
       </c>
       <c r="S6" s="50">
         <f>F6+ScoringParams!F6</f>
-        <v>-0.35</v>
+        <v>-0.17</v>
       </c>
       <c r="T6" s="41">
         <f>G6+ScoringParams!G6</f>
-        <v>-0.08</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="U6" s="41">
         <f>H6+ScoringParams!H6</f>
-        <v>-2.52</v>
+        <v>-0.31</v>
       </c>
       <c r="V6" s="41">
         <f>I6+ScoringParams!I6</f>
-        <v>-1.75</v>
+        <v>-0.22</v>
       </c>
       <c r="W6" s="41">
         <f>J6+ScoringParams!J6</f>
-        <v>-3.14</v>
+        <v>-0.09</v>
       </c>
       <c r="X6" s="50">
         <f>K6+ScoringParams!K6</f>
-        <v>-0.9</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="Y6" s="50">
         <f>L6+ScoringParams!L6</f>
-        <v>-3.5</v>
+        <v>-3.25</v>
       </c>
       <c r="Z6" s="50">
         <f>M6+ScoringParams!M6</f>
-        <v>-0.6399999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="AA6" s="51">
         <f>N6+ScoringParams!N6</f>
-        <v>-1.5899999999999999</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -2580,7 +2754,7 @@
       </c>
       <c r="S7" s="46">
         <f>F7+ScoringParams!F7</f>
-        <v>-3.4200000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="T7" s="61">
         <f>G7+ScoringParams!G7</f>
@@ -2642,7 +2816,7 @@
       </c>
       <c r="P9" s="82">
         <f>C9+ScoringParams!C17</f>
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
@@ -2657,7 +2831,7 @@
       </c>
       <c r="P10" s="83">
         <f>C10+ScoringParams!C18</f>
-        <v>-0.47499999999999998</v>
+        <v>-0.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>